<commit_message>
Add Employee Ev per segment UI
</commit_message>
<xml_diff>
--- a/src/assets/GSMs.xlsx
+++ b/src/assets/GSMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFS\Syriatel\PCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F4A49-55BA-4282-BF76-E13B52F97A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65278330-A478-4916-BD36-A2E8628BD675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{270DF063-4D78-4A52-8DA2-A7D9B87D9F57}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>GSM</t>
   </si>
@@ -140,6 +140,66 @@
   </si>
   <si>
     <t>Initialize</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -534,7 +594,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,19 +620,19 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -635,160 +695,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B0961B-323E-46CE-8D19-54C9F1C4CDE7}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>